<commit_message>
Dampf und Eis gemacht, kleine Korrekturen
</commit_message>
<xml_diff>
--- a/Versuch9/datasets/kalorimeter.xlsx
+++ b/Versuch9/datasets/kalorimeter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Documents\Uni\Grundpraktikum\Grundpraktikum\Versuch9\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{903A3C37-D596-4700-A5AF-EB6D6D3016A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{121926DB-1B02-4448-A5A3-486DC57EB438}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10920" firstSheet="2" activeTab="3" xr2:uid="{6E7FE19B-C7F4-43FF-BE23-B514B346659D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10920" firstSheet="3" activeTab="3" xr2:uid="{6E7FE19B-C7F4-43FF-BE23-B514B346659D}"/>
   </bookViews>
   <sheets>
     <sheet name="Wasserwert" sheetId="1" r:id="rId1"/>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23057D4-3AA6-4766-A7D5-A3EBAE819EF9}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3114,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBA88CE-8E4D-406B-8775-B6D57D7FDB6D}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>